<commit_message>
changing datefield models to only create date
</commit_message>
<xml_diff>
--- a/updated_inventory_list.xlsx
+++ b/updated_inventory_list.xlsx
@@ -1049,11 +1049,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1411,14 +1413,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
@@ -1438,7 +1440,7 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1482,17 +1484,17 @@
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>13.85</v>
       </c>
       <c r="C2" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F2" s="5">
+        <v>43292</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
@@ -1520,17 +1522,17 @@
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>32</v>
       </c>
       <c r="C3" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F3" s="5">
+        <v>43292</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -1558,17 +1560,17 @@
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>3.3</v>
       </c>
       <c r="C4" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F4" s="5">
+        <v>43292</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -1596,17 +1598,17 @@
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>14.5</v>
       </c>
       <c r="C5" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F5" s="5">
+        <v>43292</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -1634,17 +1636,17 @@
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>3.3</v>
       </c>
       <c r="C6" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F6" s="5">
+        <v>43292</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -1672,17 +1674,17 @@
       <c r="A7" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>27</v>
       </c>
       <c r="C7" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F7" s="5">
+        <v>43292</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -1710,14 +1712,17 @@
       <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>14</v>
       </c>
       <c r="C8" s="2">
-        <v>43263</v>
+        <v>43292</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>43292</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -1745,17 +1750,17 @@
       <c r="A9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>11</v>
       </c>
       <c r="C9" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F9" s="5">
+        <v>43292</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -1783,17 +1788,17 @@
       <c r="A10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>11</v>
       </c>
       <c r="C10" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F10" s="5">
+        <v>43292</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -1821,17 +1826,17 @@
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="4">
         <v>11</v>
       </c>
       <c r="C11" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F11" s="5">
+        <v>43292</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1859,17 +1864,17 @@
       <c r="A12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="4">
         <v>100</v>
       </c>
       <c r="C12" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F12" s="5">
+        <v>43292</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -1897,17 +1902,17 @@
       <c r="A13" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="4">
         <v>25.61</v>
       </c>
       <c r="C13" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F13" s="5">
+        <v>43292</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -1935,17 +1940,17 @@
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>11</v>
       </c>
       <c r="C14" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
       </c>
-      <c r="F14" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F14" s="5">
+        <v>43292</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -1973,17 +1978,17 @@
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="4">
         <v>85.04</v>
       </c>
       <c r="C15" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F15" s="5">
+        <v>43292</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -2011,17 +2016,17 @@
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="4">
         <v>24</v>
       </c>
       <c r="C16" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F16" s="5">
+        <v>43292</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
@@ -2049,17 +2054,17 @@
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="4">
         <v>31</v>
       </c>
       <c r="C17" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F17" s="5">
+        <v>43292</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
@@ -2087,17 +2092,17 @@
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="4">
         <v>25</v>
       </c>
       <c r="C18" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
       </c>
-      <c r="F18" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F18" s="5">
+        <v>43292</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
@@ -2125,17 +2130,17 @@
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="4">
         <v>19.25</v>
       </c>
       <c r="C19" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
       </c>
-      <c r="F19" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F19" s="5">
+        <v>43292</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
@@ -2166,17 +2171,17 @@
       <c r="A20" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
       </c>
-      <c r="F20" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F20" s="5">
+        <v>43292</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -2207,17 +2212,17 @@
       <c r="A21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="4">
         <v>9</v>
       </c>
       <c r="C21" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
       </c>
-      <c r="F21" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F21" s="5">
+        <v>43292</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
@@ -2248,17 +2253,17 @@
       <c r="A22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="4">
         <v>11</v>
       </c>
       <c r="C22" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
-      <c r="F22" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F22" s="5">
+        <v>43292</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
@@ -2286,17 +2291,17 @@
       <c r="A23" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="4">
         <v>50</v>
       </c>
       <c r="C23" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
       </c>
-      <c r="F23" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F23" s="5">
+        <v>43292</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
@@ -2324,17 +2329,17 @@
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="4">
         <v>14</v>
       </c>
       <c r="C24" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
       </c>
-      <c r="F24" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F24" s="5">
+        <v>43292</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -2362,17 +2367,17 @@
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="4">
         <v>7</v>
       </c>
       <c r="C25" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
       </c>
-      <c r="F25" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F25" s="5">
+        <v>43292</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
@@ -2403,17 +2408,17 @@
       <c r="A26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="4">
         <v>31</v>
       </c>
       <c r="C26" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
-      <c r="F26" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F26" s="5">
+        <v>43292</v>
       </c>
       <c r="G26" s="1">
         <v>0</v>
@@ -2441,17 +2446,17 @@
       <c r="A27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="4">
         <v>24</v>
       </c>
       <c r="C27" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
-      <c r="F27" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F27" s="5">
+        <v>43292</v>
       </c>
       <c r="G27" s="1">
         <v>0</v>
@@ -2479,17 +2484,17 @@
       <c r="A28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="4">
         <v>20</v>
       </c>
       <c r="C28" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
-      <c r="F28" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F28" s="5">
+        <v>43292</v>
       </c>
       <c r="G28" s="1">
         <v>0</v>
@@ -2517,17 +2522,17 @@
       <c r="A29" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="4">
         <v>17</v>
       </c>
       <c r="C29" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
-      <c r="F29" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F29" s="5">
+        <v>43292</v>
       </c>
       <c r="G29" s="1">
         <v>0</v>
@@ -2555,17 +2560,17 @@
       <c r="A30" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="4">
         <v>39.75</v>
       </c>
       <c r="C30" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
-      <c r="F30" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F30" s="5">
+        <v>43292</v>
       </c>
       <c r="G30" s="1">
         <v>0</v>
@@ -2593,17 +2598,17 @@
       <c r="A31" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="4">
         <v>144</v>
       </c>
       <c r="C31" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
       </c>
-      <c r="F31" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F31" s="5">
+        <v>43292</v>
       </c>
       <c r="G31" s="1">
         <v>0</v>
@@ -2631,17 +2636,17 @@
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="4">
         <v>72</v>
       </c>
       <c r="C32" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
-      <c r="F32" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F32" s="5">
+        <v>43292</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
@@ -2669,17 +2674,17 @@
       <c r="A33" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="4">
         <v>63</v>
       </c>
       <c r="C33" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
-      <c r="F33" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F33" s="5">
+        <v>43292</v>
       </c>
       <c r="G33" s="1">
         <v>0</v>
@@ -2710,17 +2715,17 @@
       <c r="A34" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="4">
         <v>35.75</v>
       </c>
       <c r="C34" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
       </c>
-      <c r="F34" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F34" s="5">
+        <v>43292</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
@@ -2748,17 +2753,17 @@
       <c r="A35" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="4">
         <v>20.25</v>
       </c>
       <c r="C35" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
-      <c r="F35" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F35" s="5">
+        <v>43292</v>
       </c>
       <c r="G35" s="1">
         <v>0</v>
@@ -2786,17 +2791,17 @@
       <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="4">
         <v>28</v>
       </c>
       <c r="C36" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E36" s="1">
         <v>0</v>
       </c>
-      <c r="F36" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F36" s="5">
+        <v>43292</v>
       </c>
       <c r="G36" s="1">
         <v>0</v>
@@ -2824,17 +2829,17 @@
       <c r="A37" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="4">
         <v>58</v>
       </c>
       <c r="C37" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E37" s="1">
         <v>0</v>
       </c>
-      <c r="F37" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F37" s="5">
+        <v>43292</v>
       </c>
       <c r="G37" s="1">
         <v>0</v>
@@ -2865,17 +2870,17 @@
       <c r="A38" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="4">
         <v>53</v>
       </c>
       <c r="C38" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
       </c>
-      <c r="F38" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F38" s="5">
+        <v>43292</v>
       </c>
       <c r="G38" s="1">
         <v>0</v>
@@ -2903,17 +2908,17 @@
       <c r="A39" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="4">
         <v>20</v>
       </c>
       <c r="C39" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E39" s="1">
         <v>0</v>
       </c>
-      <c r="F39" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F39" s="5">
+        <v>43292</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
@@ -2941,17 +2946,17 @@
       <c r="A40" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="4">
         <v>63</v>
       </c>
       <c r="C40" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E40" s="1">
         <v>0</v>
       </c>
-      <c r="F40" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F40" s="5">
+        <v>43292</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
@@ -2979,17 +2984,17 @@
       <c r="A41" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="4">
         <v>7</v>
       </c>
       <c r="C41" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E41" s="1">
         <v>0</v>
       </c>
-      <c r="F41" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F41" s="5">
+        <v>43292</v>
       </c>
       <c r="G41" s="1">
         <v>0</v>
@@ -3017,17 +3022,17 @@
       <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="4">
         <v>24</v>
       </c>
       <c r="C42" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E42" s="1">
         <v>0</v>
       </c>
-      <c r="F42" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F42" s="5">
+        <v>43292</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
@@ -3055,11 +3060,17 @@
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="4">
         <v>14</v>
       </c>
+      <c r="C43" s="2">
+        <v>43292</v>
+      </c>
       <c r="E43" s="1">
         <v>0</v>
+      </c>
+      <c r="F43" s="5">
+        <v>43292</v>
       </c>
       <c r="G43" s="1">
         <v>0</v>
@@ -3087,17 +3098,17 @@
       <c r="A44" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="4">
         <v>47.5</v>
       </c>
       <c r="C44" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E44" s="1">
         <v>0</v>
       </c>
-      <c r="F44" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F44" s="5">
+        <v>43292</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
@@ -3125,17 +3136,17 @@
       <c r="A45" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="4">
         <v>24</v>
       </c>
       <c r="C45" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E45" s="1">
         <v>0</v>
       </c>
-      <c r="F45" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F45" s="5">
+        <v>43292</v>
       </c>
       <c r="G45" s="1">
         <v>0</v>
@@ -3163,17 +3174,17 @@
       <c r="A46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="4">
         <v>5.23</v>
       </c>
       <c r="C46" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E46" s="1">
         <v>0</v>
       </c>
-      <c r="F46" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F46" s="5">
+        <v>43292</v>
       </c>
       <c r="G46" s="1">
         <v>0</v>
@@ -3204,17 +3215,17 @@
       <c r="A47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="4">
         <v>11.5</v>
       </c>
       <c r="C47" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E47" s="1">
         <v>0</v>
       </c>
-      <c r="F47" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F47" s="5">
+        <v>43292</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
@@ -3245,17 +3256,17 @@
       <c r="A48" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="4">
         <v>5.75</v>
       </c>
       <c r="C48" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E48" s="1">
         <v>0</v>
       </c>
-      <c r="F48" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F48" s="5">
+        <v>43292</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
@@ -3286,17 +3297,17 @@
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="4">
         <v>10</v>
       </c>
       <c r="C49" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E49" s="1">
         <v>0</v>
       </c>
-      <c r="F49" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F49" s="5">
+        <v>43292</v>
       </c>
       <c r="G49" s="1">
         <v>0</v>
@@ -3327,17 +3338,17 @@
       <c r="A50" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="4">
         <v>9</v>
       </c>
       <c r="C50" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E50" s="1">
         <v>0</v>
       </c>
-      <c r="F50" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F50" s="5">
+        <v>43292</v>
       </c>
       <c r="G50" s="1">
         <v>0</v>
@@ -3368,17 +3379,17 @@
       <c r="A51" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="4">
         <v>9</v>
       </c>
       <c r="C51" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E51" s="1">
         <v>0</v>
       </c>
-      <c r="F51" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F51" s="5">
+        <v>43292</v>
       </c>
       <c r="G51" s="1">
         <v>0</v>
@@ -3409,17 +3420,17 @@
       <c r="A52" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="4">
         <v>9</v>
       </c>
       <c r="C52" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E52" s="1">
         <v>0</v>
       </c>
-      <c r="F52" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F52" s="5">
+        <v>43292</v>
       </c>
       <c r="G52" s="1">
         <v>0</v>
@@ -3450,17 +3461,17 @@
       <c r="A53" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="4">
         <v>17.690000000000001</v>
       </c>
       <c r="C53" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E53" s="1">
         <v>0</v>
       </c>
-      <c r="F53" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F53" s="5">
+        <v>43292</v>
       </c>
       <c r="G53" s="1">
         <v>0</v>
@@ -3491,17 +3502,17 @@
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="4">
         <v>8.65</v>
       </c>
       <c r="C54" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E54" s="1">
         <v>0</v>
       </c>
-      <c r="F54" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F54" s="5">
+        <v>43292</v>
       </c>
       <c r="G54" s="1">
         <v>0</v>
@@ -3532,17 +3543,17 @@
       <c r="A55" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="4">
         <v>6.87</v>
       </c>
       <c r="C55" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
       </c>
-      <c r="F55" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F55" s="5">
+        <v>43292</v>
       </c>
       <c r="G55" s="1">
         <v>0</v>
@@ -3573,17 +3584,17 @@
       <c r="A56" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="4">
         <v>8.7200000000000006</v>
       </c>
       <c r="C56" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E56" s="1">
         <v>0</v>
       </c>
-      <c r="F56" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F56" s="5">
+        <v>43292</v>
       </c>
       <c r="G56" s="1">
         <v>0</v>
@@ -3614,17 +3625,17 @@
       <c r="A57" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="4">
         <v>12.22</v>
       </c>
       <c r="C57" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E57" s="1">
         <v>0</v>
       </c>
-      <c r="F57" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F57" s="5">
+        <v>43292</v>
       </c>
       <c r="G57" s="1">
         <v>0</v>
@@ -3655,17 +3666,17 @@
       <c r="A58" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="4">
         <v>7.51</v>
       </c>
       <c r="C58" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E58" s="1">
         <v>0</v>
       </c>
-      <c r="F58" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F58" s="5">
+        <v>43292</v>
       </c>
       <c r="G58" s="1">
         <v>0</v>
@@ -3696,17 +3707,17 @@
       <c r="A59" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="4">
         <v>8</v>
       </c>
       <c r="C59" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E59" s="1">
         <v>0</v>
       </c>
-      <c r="F59" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F59" s="5">
+        <v>43292</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
@@ -3737,17 +3748,17 @@
       <c r="A60" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="4">
         <v>26</v>
       </c>
       <c r="C60" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E60" s="1">
         <v>0</v>
       </c>
-      <c r="F60" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F60" s="5">
+        <v>43292</v>
       </c>
       <c r="G60" s="1">
         <v>0</v>
@@ -3775,17 +3786,17 @@
       <c r="A61" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="4">
         <v>14.5</v>
       </c>
       <c r="C61" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
       </c>
-      <c r="F61" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F61" s="5">
+        <v>43292</v>
       </c>
       <c r="G61" s="1">
         <v>0</v>
@@ -3816,17 +3827,17 @@
       <c r="A62" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="4">
         <v>18.5</v>
       </c>
       <c r="C62" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E62" s="1">
         <v>0</v>
       </c>
-      <c r="F62" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F62" s="5">
+        <v>43292</v>
       </c>
       <c r="G62" s="1">
         <v>0</v>
@@ -3857,17 +3868,17 @@
       <c r="A63" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="4">
         <v>19.5</v>
       </c>
       <c r="C63" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E63" s="1">
         <v>0</v>
       </c>
-      <c r="F63" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F63" s="5">
+        <v>43292</v>
       </c>
       <c r="G63" s="1">
         <v>0</v>
@@ -3898,17 +3909,17 @@
       <c r="A64" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="4">
         <v>40</v>
       </c>
       <c r="C64" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E64" s="1">
         <v>0</v>
       </c>
-      <c r="F64" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F64" s="5">
+        <v>43292</v>
       </c>
       <c r="G64" s="1">
         <v>0</v>
@@ -3936,17 +3947,17 @@
       <c r="A65" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="4">
         <v>22.5</v>
       </c>
       <c r="C65" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E65" s="1">
         <v>0</v>
       </c>
-      <c r="F65" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F65" s="5">
+        <v>43292</v>
       </c>
       <c r="G65" s="1">
         <v>0</v>
@@ -3974,17 +3985,17 @@
       <c r="A66" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="4">
         <v>61</v>
       </c>
       <c r="C66" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E66" s="1">
         <v>0</v>
       </c>
-      <c r="F66" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F66" s="5">
+        <v>43292</v>
       </c>
       <c r="G66" s="1">
         <v>0</v>
@@ -4012,17 +4023,17 @@
       <c r="A67" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="4">
         <v>70.75</v>
       </c>
       <c r="C67" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E67" s="1">
         <v>0</v>
       </c>
-      <c r="F67" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F67" s="5">
+        <v>43292</v>
       </c>
       <c r="G67" s="1">
         <v>0</v>
@@ -4050,17 +4061,17 @@
       <c r="A68" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="4">
         <v>20.75</v>
       </c>
       <c r="C68" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E68" s="1">
         <v>0</v>
       </c>
-      <c r="F68" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F68" s="5">
+        <v>43292</v>
       </c>
       <c r="G68" s="1">
         <v>0</v>
@@ -4088,17 +4099,17 @@
       <c r="A69" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="4">
         <v>21.5</v>
       </c>
       <c r="C69" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E69" s="1">
         <v>0</v>
       </c>
-      <c r="F69" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F69" s="5">
+        <v>43292</v>
       </c>
       <c r="G69" s="1">
         <v>0</v>
@@ -4126,14 +4137,17 @@
       <c r="A70" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="4">
         <v>14</v>
       </c>
       <c r="C70" s="2">
-        <v>43263</v>
+        <v>43292</v>
       </c>
       <c r="E70" s="1">
         <v>0</v>
+      </c>
+      <c r="F70" s="5">
+        <v>43292</v>
       </c>
       <c r="G70" s="1">
         <v>0</v>
@@ -4164,17 +4178,17 @@
       <c r="A71" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="4">
         <v>74.89</v>
       </c>
       <c r="C71" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E71" s="1">
         <v>0</v>
       </c>
-      <c r="F71" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F71" s="5">
+        <v>43292</v>
       </c>
       <c r="G71" s="1">
         <v>0</v>
@@ -4202,17 +4216,17 @@
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="4">
         <v>61</v>
       </c>
       <c r="C72" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E72" s="1">
         <v>0</v>
       </c>
-      <c r="F72" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F72" s="5">
+        <v>43292</v>
       </c>
       <c r="G72" s="1">
         <v>0</v>
@@ -4243,17 +4257,17 @@
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="4">
         <v>57.98</v>
       </c>
       <c r="C73" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E73" s="1">
         <v>0</v>
       </c>
-      <c r="F73" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F73" s="5">
+        <v>43292</v>
       </c>
       <c r="G73" s="1">
         <v>0</v>
@@ -4281,17 +4295,17 @@
       <c r="A74" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="4">
         <v>20.5</v>
       </c>
       <c r="C74" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E74" s="1">
         <v>0</v>
       </c>
-      <c r="F74" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F74" s="5">
+        <v>43292</v>
       </c>
       <c r="G74" s="1">
         <v>0</v>
@@ -4322,17 +4336,17 @@
       <c r="A75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="4">
         <v>21</v>
       </c>
       <c r="C75" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E75" s="1">
         <v>0</v>
       </c>
-      <c r="F75" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F75" s="5">
+        <v>43292</v>
       </c>
       <c r="G75" s="1">
         <v>0</v>
@@ -4363,17 +4377,17 @@
       <c r="A76" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="4">
         <v>13</v>
       </c>
       <c r="C76" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E76" s="1">
         <v>0</v>
       </c>
-      <c r="F76" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F76" s="5">
+        <v>43292</v>
       </c>
       <c r="G76" s="1">
         <v>0</v>
@@ -4404,17 +4418,17 @@
       <c r="A77" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="4">
         <v>66</v>
       </c>
       <c r="C77" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E77" s="1">
         <v>0</v>
       </c>
-      <c r="F77" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F77" s="5">
+        <v>43292</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
@@ -4442,14 +4456,17 @@
       <c r="A78" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="4">
         <v>10.35</v>
       </c>
       <c r="C78" s="2">
-        <v>43263</v>
+        <v>43292</v>
       </c>
       <c r="E78" s="1">
         <v>0</v>
+      </c>
+      <c r="F78" s="5">
+        <v>43292</v>
       </c>
       <c r="G78" s="1">
         <v>0</v>
@@ -4480,14 +4497,17 @@
       <c r="A79" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="4">
         <v>11.35</v>
       </c>
       <c r="C79" s="2">
-        <v>43263</v>
+        <v>43292</v>
       </c>
       <c r="E79" s="1">
         <v>0</v>
+      </c>
+      <c r="F79" s="5">
+        <v>43292</v>
       </c>
       <c r="G79" s="1">
         <v>0</v>
@@ -4518,17 +4538,17 @@
       <c r="A80" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="4">
         <v>36.549999999999997</v>
       </c>
       <c r="C80" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E80" s="1">
         <v>0</v>
       </c>
-      <c r="F80" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F80" s="5">
+        <v>43292</v>
       </c>
       <c r="G80" s="1">
         <v>0</v>
@@ -4556,17 +4576,17 @@
       <c r="A81" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="4">
         <v>44.75</v>
       </c>
       <c r="C81" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E81" s="1">
         <v>0</v>
       </c>
-      <c r="F81" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F81" s="5">
+        <v>43292</v>
       </c>
       <c r="G81" s="1">
         <v>0</v>
@@ -4597,17 +4617,17 @@
       <c r="A82" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="4">
         <v>36.5</v>
       </c>
       <c r="C82" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E82" s="1">
         <v>0</v>
       </c>
-      <c r="F82" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F82" s="5">
+        <v>43292</v>
       </c>
       <c r="G82" s="1">
         <v>0</v>
@@ -4638,17 +4658,17 @@
       <c r="A83" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="4">
         <v>22.9</v>
       </c>
       <c r="C83" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E83" s="1">
         <v>0</v>
       </c>
-      <c r="F83" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F83" s="5">
+        <v>43292</v>
       </c>
       <c r="G83" s="1">
         <v>0</v>
@@ -4679,17 +4699,17 @@
       <c r="A84" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="4">
         <v>100</v>
       </c>
       <c r="C84" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E84" s="1">
         <v>0</v>
       </c>
-      <c r="F84" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F84" s="5">
+        <v>43292</v>
       </c>
       <c r="G84" s="1">
         <v>0</v>
@@ -4720,17 +4740,17 @@
       <c r="A85" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="4">
         <v>42.5</v>
       </c>
       <c r="C85" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E85" s="1">
         <v>0</v>
       </c>
-      <c r="F85" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F85" s="5">
+        <v>43292</v>
       </c>
       <c r="G85" s="1">
         <v>0</v>
@@ -4761,17 +4781,17 @@
       <c r="A86" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="4">
         <v>29</v>
       </c>
       <c r="C86" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E86" s="1">
         <v>0</v>
       </c>
-      <c r="F86" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F86" s="5">
+        <v>43292</v>
       </c>
       <c r="G86" s="1">
         <v>0</v>
@@ -4802,17 +4822,17 @@
       <c r="A87" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="4">
         <v>21.5</v>
       </c>
       <c r="C87" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E87" s="1">
         <v>0</v>
       </c>
-      <c r="F87" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F87" s="5">
+        <v>43292</v>
       </c>
       <c r="G87" s="1">
         <v>0</v>
@@ -4843,17 +4863,17 @@
       <c r="A88" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="4">
         <v>26</v>
       </c>
       <c r="C88" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E88" s="1">
         <v>0</v>
       </c>
-      <c r="F88" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F88" s="5">
+        <v>43292</v>
       </c>
       <c r="G88" s="1">
         <v>0</v>
@@ -4881,17 +4901,17 @@
       <c r="A89" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="4">
         <v>96.25</v>
       </c>
       <c r="C89" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E89" s="1">
         <v>0</v>
       </c>
-      <c r="F89" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F89" s="5">
+        <v>43292</v>
       </c>
       <c r="G89" s="1">
         <v>0</v>
@@ -4919,17 +4939,17 @@
       <c r="A90" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="4">
         <v>16.5</v>
       </c>
       <c r="C90" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E90" s="1">
         <v>0</v>
       </c>
-      <c r="F90" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F90" s="5">
+        <v>43292</v>
       </c>
       <c r="G90" s="1">
         <v>0</v>
@@ -4957,17 +4977,17 @@
       <c r="A91" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="4">
         <v>9.1999999999999993</v>
       </c>
       <c r="C91" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E91" s="1">
         <v>0</v>
       </c>
-      <c r="F91" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F91" s="5">
+        <v>43292</v>
       </c>
       <c r="G91" s="1">
         <v>0</v>
@@ -4995,17 +5015,17 @@
       <c r="A92" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="4">
         <v>21</v>
       </c>
       <c r="C92" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E92" s="1">
         <v>0</v>
       </c>
-      <c r="F92" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F92" s="5">
+        <v>43292</v>
       </c>
       <c r="G92" s="1">
         <v>0</v>
@@ -5033,17 +5053,17 @@
       <c r="A93" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="4">
         <v>20.5</v>
       </c>
       <c r="C93" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E93" s="1">
         <v>0</v>
       </c>
-      <c r="F93" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F93" s="5">
+        <v>43292</v>
       </c>
       <c r="G93" s="1">
         <v>0</v>
@@ -5071,17 +5091,17 @@
       <c r="A94" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="4">
         <v>20</v>
       </c>
       <c r="C94" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E94" s="1">
         <v>0</v>
       </c>
-      <c r="F94" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F94" s="5">
+        <v>43292</v>
       </c>
       <c r="G94" s="1">
         <v>0</v>
@@ -5109,17 +5129,17 @@
       <c r="A95" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="4">
         <v>1</v>
       </c>
       <c r="C95" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E95" s="1">
         <v>0</v>
       </c>
-      <c r="F95" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F95" s="5">
+        <v>43292</v>
       </c>
       <c r="G95" s="1">
         <v>0</v>
@@ -5147,17 +5167,17 @@
       <c r="A96" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="4">
         <v>38.5</v>
       </c>
       <c r="C96" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E96" s="1">
         <v>0</v>
       </c>
-      <c r="F96" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F96" s="5">
+        <v>43292</v>
       </c>
       <c r="G96" s="1">
         <v>0</v>
@@ -5185,17 +5205,17 @@
       <c r="A97" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="4">
         <v>55</v>
       </c>
       <c r="C97" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E97" s="1">
         <v>0</v>
       </c>
-      <c r="F97" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F97" s="5">
+        <v>43292</v>
       </c>
       <c r="G97" s="1">
         <v>0</v>
@@ -5223,17 +5243,17 @@
       <c r="A98" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98" s="4">
         <v>31.25</v>
       </c>
       <c r="C98" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E98" s="1">
         <v>0</v>
       </c>
-      <c r="F98" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F98" s="5">
+        <v>43292</v>
       </c>
       <c r="G98" s="1">
         <v>0</v>
@@ -5261,17 +5281,17 @@
       <c r="A99" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="4">
         <v>50</v>
       </c>
       <c r="C99" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E99" s="1">
         <v>0</v>
       </c>
-      <c r="F99" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F99" s="5">
+        <v>43292</v>
       </c>
       <c r="G99" s="1">
         <v>0</v>
@@ -5299,17 +5319,17 @@
       <c r="A100" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="4">
         <v>35</v>
       </c>
       <c r="C100" s="2">
-        <v>42926</v>
+        <v>43292</v>
       </c>
       <c r="E100" s="1">
         <v>0</v>
       </c>
-      <c r="F100" s="3">
-        <v>6.7592592592592591E-3</v>
+      <c r="F100" s="5">
+        <v>43292</v>
       </c>
       <c r="G100" s="1">
         <v>0</v>

</xml_diff>